<commit_message>
DT-1498 removed reported count and last updated date from template and README
</commit_message>
<xml_diff>
--- a/Templates/project_collection/project_collection_template.xlsx
+++ b/Templates/project_collection/project_collection_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data collection project" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="307">
   <si>
     <t xml:space="preserve">Property name</t>
   </si>
@@ -142,18 +142,6 @@
   </si>
   <si>
     <t xml:space="preserve">(completion state)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last updated date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(yyyy/mm/dd)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reported count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(int)</t>
   </si>
   <si>
     <t xml:space="preserve">collection</t>
@@ -1083,7 +1071,7 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1271,10 +1259,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1380,22 +1368,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1417,10 +1391,10 @@
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <dataValidations count="8">
+  <dataValidations count="7">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B3" type="list">
       <formula1>values!$F$2:$F$15</formula1>
       <formula2>0</formula2>
@@ -1444,10 +1418,6 @@
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B12" type="list">
       <formula1>values!$J$2:$J$3</formula1>
       <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B13" type="none">
-      <formula1>1899/12/30</formula1>
-      <formula2>12/30/1899</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2" type="list">
       <formula1>values!$A$2:$A$120</formula1>
@@ -1492,1043 +1462,1043 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="G4" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="G5" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="H5" s="0" t="s">
         <v>83</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="H6" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="H7" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G8" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="H8" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="H9" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="H10" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="H11" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G12" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="H12" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="G13" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="H13" s="0" t="s">
         <v>131</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="H14" s="0" t="s">
         <v>136</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="H15" s="0" t="s">
         <v>141</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DT-1853 update template to reflect new field descriptions on instructions
</commit_message>
<xml_diff>
--- a/Templates/project_collection/project_collection_template.xlsx
+++ b/Templates/project_collection/project_collection_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data collection project" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="214">
   <si>
     <t xml:space="preserve">Property name</t>
   </si>
@@ -93,15 +93,21 @@
     <t xml:space="preserve">Title</t>
   </si>
   <si>
-    <t xml:space="preserve">(string)</t>
+    <t xml:space="preserve">(project title)</t>
   </si>
   <si>
     <t xml:space="preserve">Short title</t>
   </si>
   <si>
+    <t xml:space="preserve">(project short title)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Description</t>
   </si>
   <si>
+    <t xml:space="preserve">(project description)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Collection</t>
   </si>
   <si>
@@ -130,6 +136,15 @@
   </si>
   <si>
     <t xml:space="preserve">(technique)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(collection title)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(collection short title)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(collection description)</t>
   </si>
   <si>
     <t xml:space="preserve">Access control</t>
@@ -777,8 +792,8 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -897,15 +912,15 @@
         <v>24</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -963,14 +978,14 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -984,7 +999,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>15</v>
@@ -992,31 +1007,31 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>7</v>
@@ -1024,10 +1039,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1035,7 +1050,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1043,31 +1058,31 @@
         <v>24</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1145,7 +1160,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.48"/>
@@ -1159,591 +1174,591 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F35" s="0" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F36" s="0" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F37" s="0" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F38" s="0" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F39" s="0" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F40" s="0" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G41" s="0" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-updated controlled vocabs for Templates for 2021Q4
</commit_message>
<xml_diff>
--- a/Templates/project_collection/project_collection_template.xlsx
+++ b/Templates/project_collection/project_collection_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pam.baker/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pam.baker/Documents/repos/BCDC-Metadata/Templates/project_collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13F8347-1F44-E049-B581-A74D9E5D8F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B27B36E-A06E-0B4B-A05E-28049A304DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23940" windowHeight="15700" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="1720" windowWidth="16380" windowHeight="15700" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data collection project" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="232">
   <si>
     <t>Property name</t>
   </si>
@@ -702,6 +702,27 @@
   </si>
   <si>
     <t>reconstruction</t>
+  </si>
+  <si>
+    <t>10X Genomics Multiome</t>
+  </si>
+  <si>
+    <t>enhancer virus labeling</t>
+  </si>
+  <si>
+    <t>whole genome sequencing</t>
+  </si>
+  <si>
+    <t>common tree shrew</t>
+  </si>
+  <si>
+    <t>domestic cat</t>
+  </si>
+  <si>
+    <t>pig</t>
+  </si>
+  <si>
+    <t>small-eared galago</t>
   </si>
 </sst>
 </file>
@@ -720,12 +741,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1385,15 +1406,6 @@
           </x14:formula2>
           <xm:sqref>B12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
-          <x14:formula1>
-            <xm:f>values!$D$2:$D$100</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>B4</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>values!$C$2:$C$100</xm:f>
@@ -1402,15 +1414,6 @@
             <xm:f>0</xm:f>
           </x14:formula2>
           <xm:sqref>B5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
-          <x14:formula1>
-            <xm:f>values!$G$2:$G$107</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
@@ -1421,6 +1424,24 @@
           </x14:formula2>
           <xm:sqref>B3</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
+          <x14:formula1>
+            <xm:f>values!$G$2:$G$109</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>B7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
+          <x14:formula1>
+            <xm:f>values!$D$2:$D$104</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>B4</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1429,10 +1450,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1544,7 +1565,7 @@
         <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>228</v>
       </c>
       <c r="E4" t="s">
         <v>74</v>
@@ -1553,7 +1574,7 @@
         <v>75</v>
       </c>
       <c r="G4" t="s">
-        <v>76</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1564,7 +1585,7 @@
         <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
         <v>80</v>
@@ -1573,7 +1594,7 @@
         <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1584,7 +1605,7 @@
         <v>84</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>229</v>
       </c>
       <c r="E6" t="s">
         <v>86</v>
@@ -1593,7 +1614,7 @@
         <v>87</v>
       </c>
       <c r="G6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1604,7 +1625,7 @@
         <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="E7" t="s">
         <v>92</v>
@@ -1613,7 +1634,7 @@
         <v>93</v>
       </c>
       <c r="G7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1624,7 +1645,7 @@
         <v>96</v>
       </c>
       <c r="D8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E8" t="s">
         <v>98</v>
@@ -1632,8 +1653,8 @@
       <c r="F8" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>100</v>
+      <c r="G8" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1644,7 +1665,7 @@
         <v>102</v>
       </c>
       <c r="D9" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="E9" t="s">
         <v>104</v>
@@ -1652,8 +1673,8 @@
       <c r="F9" t="s">
         <v>105</v>
       </c>
-      <c r="G9" t="s">
-        <v>106</v>
+      <c r="G9" s="3" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1664,7 +1685,7 @@
         <v>108</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>222</v>
@@ -1672,8 +1693,8 @@
       <c r="F10" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>214</v>
+      <c r="G10" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1684,7 +1705,7 @@
         <v>114</v>
       </c>
       <c r="D11" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>223</v>
@@ -1693,7 +1714,7 @@
         <v>117</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1704,7 +1725,7 @@
         <v>120</v>
       </c>
       <c r="D12" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>224</v>
@@ -1712,8 +1733,8 @@
       <c r="F12" t="s">
         <v>123</v>
       </c>
-      <c r="G12" t="s">
-        <v>112</v>
+      <c r="G12" s="5" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1724,7 +1745,7 @@
         <v>126</v>
       </c>
       <c r="D13" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="E13" t="s">
         <v>110</v>
@@ -1733,7 +1754,7 @@
         <v>129</v>
       </c>
       <c r="G13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1744,7 +1765,7 @@
         <v>213</v>
       </c>
       <c r="D14" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="E14" t="s">
         <v>116</v>
@@ -1752,8 +1773,8 @@
       <c r="F14" t="s">
         <v>134</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>124</v>
+      <c r="G14" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1761,7 +1782,7 @@
         <v>136</v>
       </c>
       <c r="D15" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="E15" t="s">
         <v>122</v>
@@ -1769,8 +1790,8 @@
       <c r="F15" t="s">
         <v>139</v>
       </c>
-      <c r="G15" t="s">
-        <v>130</v>
+      <c r="G15" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1778,7 +1799,7 @@
         <v>141</v>
       </c>
       <c r="D16" t="s">
-        <v>142</v>
+        <v>230</v>
       </c>
       <c r="E16" t="s">
         <v>128</v>
@@ -1787,7 +1808,7 @@
         <v>143</v>
       </c>
       <c r="G16" t="s">
-        <v>135</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1795,7 +1816,7 @@
         <v>145</v>
       </c>
       <c r="D17" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="E17" t="s">
         <v>133</v>
@@ -1804,13 +1825,16 @@
         <v>147</v>
       </c>
       <c r="G17" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>149</v>
       </c>
+      <c r="D18" t="s">
+        <v>137</v>
+      </c>
       <c r="E18" t="s">
         <v>138</v>
       </c>
@@ -1818,40 +1842,49 @@
         <v>150</v>
       </c>
       <c r="G18" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>152</v>
       </c>
+      <c r="D19" t="s">
+        <v>142</v>
+      </c>
       <c r="F19" t="s">
         <v>153</v>
       </c>
       <c r="G19" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>155</v>
       </c>
+      <c r="D20" t="s">
+        <v>231</v>
+      </c>
       <c r="F20" t="s">
         <v>156</v>
       </c>
       <c r="G20" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>158</v>
       </c>
+      <c r="D21" t="s">
+        <v>146</v>
+      </c>
       <c r="F21" t="s">
         <v>159</v>
       </c>
       <c r="G21" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1862,7 +1895,7 @@
         <v>162</v>
       </c>
       <c r="G22" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1873,7 +1906,7 @@
         <v>165</v>
       </c>
       <c r="G23" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1884,7 +1917,7 @@
         <v>168</v>
       </c>
       <c r="G24" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1895,7 +1928,7 @@
         <v>171</v>
       </c>
       <c r="G25" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1906,7 +1939,7 @@
         <v>174</v>
       </c>
       <c r="G26" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1917,7 +1950,7 @@
         <v>177</v>
       </c>
       <c r="G27" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1928,7 +1961,7 @@
         <v>180</v>
       </c>
       <c r="G28" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1938,8 +1971,8 @@
       <c r="F29" t="s">
         <v>183</v>
       </c>
-      <c r="G29" s="5" t="s">
-        <v>216</v>
+      <c r="G29" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1949,8 +1982,8 @@
       <c r="F30" t="s">
         <v>186</v>
       </c>
-      <c r="G30" s="5" t="s">
-        <v>217</v>
+      <c r="G30" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1960,8 +1993,8 @@
       <c r="F31" t="s">
         <v>189</v>
       </c>
-      <c r="G31" t="s">
-        <v>178</v>
+      <c r="G31" s="5" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1971,8 +2004,8 @@
       <c r="F32" t="s">
         <v>192</v>
       </c>
-      <c r="G32" t="s">
-        <v>181</v>
+      <c r="G32" s="5" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1983,7 +2016,7 @@
         <v>195</v>
       </c>
       <c r="G33" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1994,31 +2027,31 @@
         <v>198</v>
       </c>
       <c r="G34" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F35" t="s">
         <v>200</v>
       </c>
-      <c r="G35" s="3" t="s">
-        <v>190</v>
+      <c r="G35" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F36" t="s">
         <v>202</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>193</v>
+      <c r="G36" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F37" t="s">
         <v>204</v>
       </c>
-      <c r="G37" t="s">
-        <v>196</v>
+      <c r="G37" s="3" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -2026,63 +2059,78 @@
         <v>205</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F39" t="s">
         <v>207</v>
       </c>
-      <c r="G39" s="3" t="s">
-        <v>201</v>
+      <c r="G39" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F40" t="s">
         <v>209</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G41" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G42" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G41" s="6" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G43" s="6" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G42" s="5" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G44" s="5" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G43" s="5" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G45" s="5" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G44" s="6" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G46" s="6" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G45" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G46" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G47" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G48" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G49" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G50" t="s">
         <v>211</v>
+      </c>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G51" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-updated controlled vocabs for 2021Q4
</commit_message>
<xml_diff>
--- a/Templates/project_collection/project_collection_template.xlsx
+++ b/Templates/project_collection/project_collection_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pam.baker/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pam.baker/Documents/repos/BCDC-Metadata/Templates/project_collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13F8347-1F44-E049-B581-A74D9E5D8F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B27B36E-A06E-0B4B-A05E-28049A304DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23940" windowHeight="15700" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="1720" windowWidth="16380" windowHeight="15700" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data collection project" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="232">
   <si>
     <t>Property name</t>
   </si>
@@ -702,6 +702,27 @@
   </si>
   <si>
     <t>reconstruction</t>
+  </si>
+  <si>
+    <t>10X Genomics Multiome</t>
+  </si>
+  <si>
+    <t>enhancer virus labeling</t>
+  </si>
+  <si>
+    <t>whole genome sequencing</t>
+  </si>
+  <si>
+    <t>common tree shrew</t>
+  </si>
+  <si>
+    <t>domestic cat</t>
+  </si>
+  <si>
+    <t>pig</t>
+  </si>
+  <si>
+    <t>small-eared galago</t>
   </si>
 </sst>
 </file>
@@ -720,12 +741,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1385,15 +1406,6 @@
           </x14:formula2>
           <xm:sqref>B12</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
-          <x14:formula1>
-            <xm:f>values!$D$2:$D$100</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>B4</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>values!$C$2:$C$100</xm:f>
@@ -1402,15 +1414,6 @@
             <xm:f>0</xm:f>
           </x14:formula2>
           <xm:sqref>B5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
-          <x14:formula1>
-            <xm:f>values!$G$2:$G$107</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
@@ -1421,6 +1424,24 @@
           </x14:formula2>
           <xm:sqref>B3</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
+          <x14:formula1>
+            <xm:f>values!$G$2:$G$109</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>B7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
+          <x14:formula1>
+            <xm:f>values!$D$2:$D$104</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>B4</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1429,10 +1450,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1544,7 +1565,7 @@
         <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>228</v>
       </c>
       <c r="E4" t="s">
         <v>74</v>
@@ -1553,7 +1574,7 @@
         <v>75</v>
       </c>
       <c r="G4" t="s">
-        <v>76</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1564,7 +1585,7 @@
         <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
         <v>80</v>
@@ -1573,7 +1594,7 @@
         <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1584,7 +1605,7 @@
         <v>84</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>229</v>
       </c>
       <c r="E6" t="s">
         <v>86</v>
@@ -1593,7 +1614,7 @@
         <v>87</v>
       </c>
       <c r="G6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1604,7 +1625,7 @@
         <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="E7" t="s">
         <v>92</v>
@@ -1613,7 +1634,7 @@
         <v>93</v>
       </c>
       <c r="G7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1624,7 +1645,7 @@
         <v>96</v>
       </c>
       <c r="D8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E8" t="s">
         <v>98</v>
@@ -1632,8 +1653,8 @@
       <c r="F8" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>100</v>
+      <c r="G8" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1644,7 +1665,7 @@
         <v>102</v>
       </c>
       <c r="D9" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="E9" t="s">
         <v>104</v>
@@ -1652,8 +1673,8 @@
       <c r="F9" t="s">
         <v>105</v>
       </c>
-      <c r="G9" t="s">
-        <v>106</v>
+      <c r="G9" s="3" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1664,7 +1685,7 @@
         <v>108</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>222</v>
@@ -1672,8 +1693,8 @@
       <c r="F10" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>214</v>
+      <c r="G10" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1684,7 +1705,7 @@
         <v>114</v>
       </c>
       <c r="D11" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>223</v>
@@ -1693,7 +1714,7 @@
         <v>117</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1704,7 +1725,7 @@
         <v>120</v>
       </c>
       <c r="D12" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>224</v>
@@ -1712,8 +1733,8 @@
       <c r="F12" t="s">
         <v>123</v>
       </c>
-      <c r="G12" t="s">
-        <v>112</v>
+      <c r="G12" s="5" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1724,7 +1745,7 @@
         <v>126</v>
       </c>
       <c r="D13" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="E13" t="s">
         <v>110</v>
@@ -1733,7 +1754,7 @@
         <v>129</v>
       </c>
       <c r="G13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1744,7 +1765,7 @@
         <v>213</v>
       </c>
       <c r="D14" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="E14" t="s">
         <v>116</v>
@@ -1752,8 +1773,8 @@
       <c r="F14" t="s">
         <v>134</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>124</v>
+      <c r="G14" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1761,7 +1782,7 @@
         <v>136</v>
       </c>
       <c r="D15" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="E15" t="s">
         <v>122</v>
@@ -1769,8 +1790,8 @@
       <c r="F15" t="s">
         <v>139</v>
       </c>
-      <c r="G15" t="s">
-        <v>130</v>
+      <c r="G15" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1778,7 +1799,7 @@
         <v>141</v>
       </c>
       <c r="D16" t="s">
-        <v>142</v>
+        <v>230</v>
       </c>
       <c r="E16" t="s">
         <v>128</v>
@@ -1787,7 +1808,7 @@
         <v>143</v>
       </c>
       <c r="G16" t="s">
-        <v>135</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1795,7 +1816,7 @@
         <v>145</v>
       </c>
       <c r="D17" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="E17" t="s">
         <v>133</v>
@@ -1804,13 +1825,16 @@
         <v>147</v>
       </c>
       <c r="G17" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>149</v>
       </c>
+      <c r="D18" t="s">
+        <v>137</v>
+      </c>
       <c r="E18" t="s">
         <v>138</v>
       </c>
@@ -1818,40 +1842,49 @@
         <v>150</v>
       </c>
       <c r="G18" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>152</v>
       </c>
+      <c r="D19" t="s">
+        <v>142</v>
+      </c>
       <c r="F19" t="s">
         <v>153</v>
       </c>
       <c r="G19" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>155</v>
       </c>
+      <c r="D20" t="s">
+        <v>231</v>
+      </c>
       <c r="F20" t="s">
         <v>156</v>
       </c>
       <c r="G20" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>158</v>
       </c>
+      <c r="D21" t="s">
+        <v>146</v>
+      </c>
       <c r="F21" t="s">
         <v>159</v>
       </c>
       <c r="G21" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1862,7 +1895,7 @@
         <v>162</v>
       </c>
       <c r="G22" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1873,7 +1906,7 @@
         <v>165</v>
       </c>
       <c r="G23" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1884,7 +1917,7 @@
         <v>168</v>
       </c>
       <c r="G24" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1895,7 +1928,7 @@
         <v>171</v>
       </c>
       <c r="G25" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1906,7 +1939,7 @@
         <v>174</v>
       </c>
       <c r="G26" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1917,7 +1950,7 @@
         <v>177</v>
       </c>
       <c r="G27" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1928,7 +1961,7 @@
         <v>180</v>
       </c>
       <c r="G28" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1938,8 +1971,8 @@
       <c r="F29" t="s">
         <v>183</v>
       </c>
-      <c r="G29" s="5" t="s">
-        <v>216</v>
+      <c r="G29" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1949,8 +1982,8 @@
       <c r="F30" t="s">
         <v>186</v>
       </c>
-      <c r="G30" s="5" t="s">
-        <v>217</v>
+      <c r="G30" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1960,8 +1993,8 @@
       <c r="F31" t="s">
         <v>189</v>
       </c>
-      <c r="G31" t="s">
-        <v>178</v>
+      <c r="G31" s="5" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1971,8 +2004,8 @@
       <c r="F32" t="s">
         <v>192</v>
       </c>
-      <c r="G32" t="s">
-        <v>181</v>
+      <c r="G32" s="5" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1983,7 +2016,7 @@
         <v>195</v>
       </c>
       <c r="G33" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1994,31 +2027,31 @@
         <v>198</v>
       </c>
       <c r="G34" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F35" t="s">
         <v>200</v>
       </c>
-      <c r="G35" s="3" t="s">
-        <v>190</v>
+      <c r="G35" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F36" t="s">
         <v>202</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>193</v>
+      <c r="G36" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F37" t="s">
         <v>204</v>
       </c>
-      <c r="G37" t="s">
-        <v>196</v>
+      <c r="G37" s="3" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -2026,63 +2059,78 @@
         <v>205</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F39" t="s">
         <v>207</v>
       </c>
-      <c r="G39" s="3" t="s">
-        <v>201</v>
+      <c r="G39" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F40" t="s">
         <v>209</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G41" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G42" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G41" s="6" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G43" s="6" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G42" s="5" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G44" s="5" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G43" s="5" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G45" s="5" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G44" s="6" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G46" s="6" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G45" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G46" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G47" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G48" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G49" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G50" t="s">
         <v>211</v>
+      </c>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G51" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated template for 2022Q3
</commit_message>
<xml_diff>
--- a/Templates/project_collection/project_collection_template.xlsx
+++ b/Templates/project_collection/project_collection_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pam.baker/Documents/repos/BCDC-Metadata/Templates/project_collection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pam.baker/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B27B36E-A06E-0B4B-A05E-28049A304DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE47088-9569-C24B-AFB2-FCC6322AEB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="1720" windowWidth="16380" windowHeight="15700" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="1720" windowWidth="22480" windowHeight="15700" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data collection project" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="242">
   <si>
     <t>Property name</t>
   </si>
@@ -518,9 +518,6 @@
     <t>TransChar</t>
   </si>
   <si>
-    <t>mouselight</t>
-  </si>
-  <si>
     <t>U01 Kriegstein grant</t>
   </si>
   <si>
@@ -723,6 +720,39 @@
   </si>
   <si>
     <t>small-eared galago</t>
+  </si>
+  <si>
+    <t>RF1 Adey grant</t>
+  </si>
+  <si>
+    <t>RF1 Shepherd</t>
+  </si>
+  <si>
+    <t>RF1 Kim grant</t>
+  </si>
+  <si>
+    <t>RF1 Ren grant</t>
+  </si>
+  <si>
+    <t>10x Chromium 3' v3.1 sequencing</t>
+  </si>
+  <si>
+    <t>gwas</t>
+  </si>
+  <si>
+    <t>MouseLight</t>
+  </si>
+  <si>
+    <t>Oxford Nanopore long read sequencing</t>
+  </si>
+  <si>
+    <t>PacBio long read sequencing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sci-ATAC-v3 </t>
+  </si>
+  <si>
+    <t>TempO-seq</t>
   </si>
 </sst>
 </file>
@@ -1258,7 +1288,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
-            <xm:f>values!$A$2:$A$100</xm:f>
+            <xm:f>values!$A$2:$A$104</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
@@ -1424,15 +1454,6 @@
           </x14:formula2>
           <xm:sqref>B3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
-          <x14:formula1>
-            <xm:f>values!$G$2:$G$109</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>B7</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>values!$D$2:$D$104</xm:f>
@@ -1442,6 +1463,15 @@
           </x14:formula2>
           <xm:sqref>B4</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
+          <x14:formula1>
+            <xm:f>values!$G$2:$G$115</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>B7</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1450,10 +1480,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1507,7 +1537,7 @@
         <v>55</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -1565,7 +1595,7 @@
         <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E4" t="s">
         <v>74</v>
@@ -1574,7 +1604,7 @@
         <v>75</v>
       </c>
       <c r="G4" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1594,7 +1624,7 @@
         <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>76</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1605,7 +1635,7 @@
         <v>84</v>
       </c>
       <c r="D6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E6" t="s">
         <v>86</v>
@@ -1614,7 +1644,7 @@
         <v>87</v>
       </c>
       <c r="G6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1634,7 +1664,7 @@
         <v>93</v>
       </c>
       <c r="G7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1654,7 +1684,7 @@
         <v>99</v>
       </c>
       <c r="G8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1673,13 +1703,13 @@
       <c r="F9" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>100</v>
+      <c r="G9" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>107</v>
+        <v>231</v>
       </c>
       <c r="C10" t="s">
         <v>108</v>
@@ -1688,18 +1718,18 @@
         <v>97</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F10" t="s">
         <v>111</v>
       </c>
-      <c r="G10" t="s">
-        <v>106</v>
+      <c r="G10" s="3" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C11" t="s">
         <v>114</v>
@@ -1708,18 +1738,18 @@
         <v>103</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F11" t="s">
         <v>117</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>214</v>
+      <c r="G11" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>119</v>
+        <v>233</v>
       </c>
       <c r="C12" t="s">
         <v>120</v>
@@ -1728,18 +1758,18 @@
         <v>109</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F12" t="s">
         <v>123</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C13" t="s">
         <v>126</v>
@@ -1753,16 +1783,16 @@
       <c r="F13" t="s">
         <v>129</v>
       </c>
-      <c r="G13" t="s">
-        <v>112</v>
+      <c r="G13" s="5" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D14" t="s">
         <v>121</v>
@@ -1774,12 +1804,12 @@
         <v>134</v>
       </c>
       <c r="G14" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D15" t="s">
         <v>127</v>
@@ -1790,16 +1820,16 @@
       <c r="F15" t="s">
         <v>139</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>124</v>
+      <c r="G15" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E16" t="s">
         <v>128</v>
@@ -1807,13 +1837,13 @@
       <c r="F16" t="s">
         <v>143</v>
       </c>
-      <c r="G16" t="s">
-        <v>226</v>
+      <c r="G16" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>145</v>
+        <v>234</v>
       </c>
       <c r="D17" t="s">
         <v>132</v>
@@ -1825,12 +1855,12 @@
         <v>147</v>
       </c>
       <c r="G17" t="s">
-        <v>130</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>149</v>
+        <v>232</v>
       </c>
       <c r="D18" t="s">
         <v>137</v>
@@ -1842,12 +1872,12 @@
         <v>150</v>
       </c>
       <c r="G18" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="D19" t="s">
         <v>142</v>
@@ -1856,26 +1886,26 @@
         <v>153</v>
       </c>
       <c r="G19" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="D20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F20" t="s">
         <v>156</v>
       </c>
       <c r="G20" t="s">
-        <v>144</v>
+        <v>236</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="D21" t="s">
         <v>146</v>
@@ -1884,253 +1914,295 @@
         <v>159</v>
       </c>
       <c r="G21" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="F22" t="s">
         <v>162</v>
       </c>
       <c r="G22" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>152</v>
+      </c>
+      <c r="F23" t="s">
         <v>164</v>
       </c>
-      <c r="F23" t="s">
-        <v>165</v>
-      </c>
       <c r="G23" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>155</v>
+      </c>
+      <c r="F24" t="s">
         <v>167</v>
       </c>
-      <c r="F24" t="s">
-        <v>168</v>
-      </c>
       <c r="G24" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>158</v>
+      </c>
+      <c r="F25" t="s">
         <v>170</v>
       </c>
-      <c r="F25" t="s">
-        <v>171</v>
-      </c>
       <c r="G25" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>161</v>
+      </c>
+      <c r="F26" t="s">
         <v>173</v>
       </c>
-      <c r="F26" t="s">
-        <v>174</v>
-      </c>
       <c r="G26" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>163</v>
+      </c>
+      <c r="F27" t="s">
         <v>176</v>
       </c>
-      <c r="F27" t="s">
-        <v>177</v>
-      </c>
       <c r="G27" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>166</v>
+      </c>
+      <c r="F28" t="s">
         <v>179</v>
       </c>
-      <c r="F28" t="s">
-        <v>180</v>
-      </c>
       <c r="G28" t="s">
-        <v>169</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>169</v>
+      </c>
+      <c r="F29" t="s">
         <v>182</v>
       </c>
-      <c r="F29" t="s">
-        <v>183</v>
-      </c>
       <c r="G29" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>172</v>
+      </c>
+      <c r="F30" t="s">
         <v>185</v>
       </c>
-      <c r="F30" t="s">
-        <v>186</v>
-      </c>
       <c r="G30" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>175</v>
+      </c>
+      <c r="F31" t="s">
         <v>188</v>
       </c>
-      <c r="F31" t="s">
-        <v>189</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>216</v>
+      <c r="G31" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>178</v>
+      </c>
+      <c r="F32" t="s">
         <v>191</v>
       </c>
-      <c r="F32" t="s">
-        <v>192</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>217</v>
+      <c r="G32" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>181</v>
+      </c>
+      <c r="F33" t="s">
         <v>194</v>
       </c>
-      <c r="F33" t="s">
-        <v>195</v>
-      </c>
-      <c r="G33" t="s">
-        <v>178</v>
+      <c r="G33" s="5" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>184</v>
+      </c>
+      <c r="F34" t="s">
         <v>197</v>
       </c>
-      <c r="F34" t="s">
-        <v>198</v>
-      </c>
-      <c r="G34" t="s">
-        <v>181</v>
+      <c r="G34" s="5" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>187</v>
+      </c>
       <c r="F35" t="s">
-        <v>200</v>
-      </c>
-      <c r="G35" t="s">
-        <v>184</v>
+        <v>199</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>190</v>
+      </c>
       <c r="F36" t="s">
-        <v>202</v>
-      </c>
-      <c r="G36" t="s">
-        <v>187</v>
+        <v>201</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>193</v>
+      </c>
       <c r="F37" t="s">
+        <v>203</v>
+      </c>
+      <c r="G37" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>196</v>
+      </c>
+      <c r="F38" t="s">
         <v>204</v>
       </c>
-      <c r="G37" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F38" t="s">
-        <v>205</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>193</v>
+      <c r="G38" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F39" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G39" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F40" t="s">
-        <v>209</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>199</v>
+        <v>208</v>
+      </c>
+      <c r="G40" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G41" s="3" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G42" t="s">
-        <v>203</v>
+      <c r="G42" s="3" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G43" s="6" t="s">
-        <v>218</v>
+      <c r="G43" s="3" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G44" s="5" t="s">
-        <v>219</v>
+      <c r="G44" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G45" s="5" t="s">
-        <v>220</v>
+      <c r="G45" s="3" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G46" s="6" t="s">
-        <v>221</v>
+      <c r="G46" s="3" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G47" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G48" t="s">
-        <v>208</v>
+      <c r="G48" s="6" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G49" t="s">
+      <c r="G49" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G50" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G51" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="52" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G52" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="53" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G53" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="54" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G54" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="55" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G55" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="56" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G56" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G50" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G51" t="s">
-        <v>227</v>
+    <row r="57" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G57" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>